<commit_message>
atualizando o nome e fazendo pesquisa abranger codigo e nomes sem acentos
</commit_message>
<xml_diff>
--- a/exames.xlsx
+++ b/exames.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\bigFarma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43C6909D-2301-4E14-A0CD-159E988148AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDCD26C6-E725-4BC9-9618-457731742221}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2517,10 +2517,10 @@
     <t>URI EAS</t>
   </si>
   <si>
-    <t>HOMÔNIMO FOLÍCULO ESTIMULANTE</t>
-  </si>
-  <si>
     <t>FSH</t>
+  </si>
+  <si>
+    <t>HORMÔNIO FOLÍCULO ESTIMULANTE</t>
   </si>
 </sst>
 </file>
@@ -2616,7 +2616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2666,12 +2666,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -2979,10 +2982,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D413"/>
+  <dimension ref="A1:M413"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A371" workbookViewId="0">
-      <selection activeCell="B413" sqref="B413"/>
+    <sheetView tabSelected="1" topLeftCell="A367" workbookViewId="0">
+      <selection activeCell="M403" sqref="M403"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3000,10 +3003,10 @@
       <c r="B1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="16"/>
+      <c r="D1" s="18"/>
     </row>
     <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -8587,7 +8590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="401" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A401" s="3" t="s">
         <v>300</v>
       </c>
@@ -8601,7 +8604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="402" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A402" s="3" t="s">
         <v>306</v>
       </c>
@@ -8615,7 +8618,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="403" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A403" s="3" t="s">
         <v>314</v>
       </c>
@@ -8628,8 +8631,9 @@
       <c r="D403" s="12">
         <v>15</v>
       </c>
-    </row>
-    <row r="404" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="M403" s="19"/>
+    </row>
+    <row r="404" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A404" s="3" t="s">
         <v>328</v>
       </c>
@@ -8643,7 +8647,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="405" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A405" s="3" t="s">
         <v>346</v>
       </c>
@@ -8657,7 +8661,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="406" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A406" s="3" t="s">
         <v>732</v>
       </c>
@@ -8671,7 +8675,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="407" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A407" s="3" t="s">
         <v>734</v>
       </c>
@@ -8685,7 +8689,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="408" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A408" s="3" t="s">
         <v>769</v>
       </c>
@@ -8699,7 +8703,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="409" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A409" s="3" t="s">
         <v>742</v>
       </c>
@@ -8713,12 +8717,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="410" spans="1:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="A410" s="17" t="s">
+    <row r="410" spans="1:13" ht="15" x14ac:dyDescent="0.2">
+      <c r="A410" s="16" t="s">
+        <v>815</v>
+      </c>
+      <c r="B410" s="16" t="s">
         <v>816</v>
-      </c>
-      <c r="B410" s="17" t="s">
-        <v>815</v>
       </c>
       <c r="C410" s="4">
         <v>50</v>
@@ -8727,8 +8731,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B413" s="18"/>
+    <row r="413" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B413" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>